<commit_message>
BCOP3561 Import Market Coverages: updated market coverages file in order to save coverages successfully
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Market coverages.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Market coverages.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="555" yWindow="555" windowWidth="25035" windowHeight="15615" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,9 +374,6 @@
     <t>Augusta-Aiken</t>
   </si>
   <si>
-    <t>Fargo</t>
-  </si>
-  <si>
     <t>Yakima-Pasco-Rchlnd-Knnwck</t>
   </si>
   <si>
@@ -621,9 +623,6 @@
     <t>San Angelo</t>
   </si>
   <si>
-    <t>Cheyenne-Scottsbluff</t>
-  </si>
-  <si>
     <t>Casper-Riverton</t>
   </si>
   <si>
@@ -664,16 +663,22 @@
   </si>
   <si>
     <t>NSI Total U.S.</t>
+  </si>
+  <si>
+    <t>Fargo-Valley City</t>
+  </si>
+  <si>
+    <t>Cheyenne-Scottsbluf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -729,10 +734,18 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1060,11 +1073,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D212"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="39" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -2653,7 +2669,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
       <c r="C114" s="5">
         <v>240560</v>
@@ -2667,7 +2683,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C115" s="5">
         <v>239760</v>
@@ -2681,7 +2697,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C116" s="5">
         <v>238990</v>
@@ -2695,7 +2711,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C117" s="5">
         <v>237580</v>
@@ -2709,7 +2725,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C118" s="5">
         <v>234120</v>
@@ -2723,7 +2739,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C119" s="5">
         <v>233370</v>
@@ -2737,7 +2753,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C120" s="5">
         <v>231570</v>
@@ -2751,7 +2767,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C121" s="5">
         <v>222970</v>
@@ -2765,7 +2781,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C122" s="5">
         <v>222450</v>
@@ -2779,7 +2795,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C123" s="5">
         <v>222210</v>
@@ -2793,7 +2809,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C124" s="5">
         <v>222190</v>
@@ -2807,7 +2823,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C125" s="5">
         <v>218740</v>
@@ -2821,7 +2837,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C126" s="5">
         <v>217560</v>
@@ -2835,7 +2851,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C127" s="5">
         <v>212180</v>
@@ -2849,7 +2865,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C128" s="5">
         <v>206520</v>
@@ -2863,7 +2879,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C129" s="5">
         <v>198820</v>
@@ -2877,7 +2893,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C130" s="5">
         <v>196160</v>
@@ -2891,7 +2907,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C131" s="5">
         <v>191440</v>
@@ -2905,7 +2921,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C132" s="5">
         <v>179920</v>
@@ -2919,7 +2935,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C133" s="5">
         <v>179370</v>
@@ -2933,7 +2949,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C134" s="5">
         <v>172520</v>
@@ -2947,7 +2963,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C135" s="5">
         <v>166030</v>
@@ -2961,7 +2977,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C136" s="5">
         <v>163790</v>
@@ -2975,7 +2991,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C137" s="5">
         <v>163600</v>
@@ -2989,7 +3005,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C138" s="5">
         <v>161950</v>
@@ -3003,7 +3019,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C139" s="5">
         <v>161530</v>
@@ -3017,7 +3033,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C140" s="5">
         <v>161010</v>
@@ -3031,7 +3047,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C141" s="5">
         <v>157070</v>
@@ -3045,7 +3061,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C142" s="5">
         <v>156240</v>
@@ -3059,7 +3075,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C143" s="5">
         <v>156020</v>
@@ -3073,7 +3089,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C144" s="5">
         <v>155240</v>
@@ -3087,7 +3103,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C145" s="5">
         <v>153830</v>
@@ -3101,7 +3117,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C146" s="5">
         <v>153370</v>
@@ -3115,7 +3131,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C147" s="5">
         <v>152840</v>
@@ -3129,7 +3145,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C148" s="5">
         <v>149120</v>
@@ -3143,7 +3159,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C149" s="5">
         <v>144180</v>
@@ -3157,7 +3173,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C150" s="5">
         <v>142990</v>
@@ -3171,7 +3187,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C151" s="5">
         <v>141020</v>
@@ -3185,7 +3201,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C152" s="5">
         <v>137830</v>
@@ -3199,7 +3215,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C153" s="5">
         <v>136740</v>
@@ -3213,7 +3229,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C154" s="5">
         <v>134990</v>
@@ -3227,7 +3243,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C155" s="5">
         <v>134510</v>
@@ -3241,7 +3257,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C156" s="5">
         <v>127470</v>
@@ -3255,7 +3271,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C157" s="5">
         <v>125970</v>
@@ -3269,7 +3285,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C158" s="5">
         <v>124130</v>
@@ -3283,7 +3299,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C159" s="5">
         <v>121320</v>
@@ -3297,7 +3313,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C160" s="5">
         <v>121060</v>
@@ -3311,7 +3327,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C161" s="5">
         <v>120100</v>
@@ -3325,7 +3341,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C162" s="5">
         <v>120060</v>
@@ -3339,7 +3355,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C163" s="5">
         <v>119590</v>
@@ -3353,7 +3369,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C164" s="5">
         <v>118520</v>
@@ -3367,7 +3383,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C165" s="5">
         <v>113110</v>
@@ -3381,7 +3397,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C166" s="5">
         <v>107760</v>
@@ -3395,7 +3411,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C167" s="5">
         <v>105690</v>
@@ -3409,7 +3425,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C168" s="5">
         <v>105470</v>
@@ -3423,7 +3439,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C169" s="5">
         <v>102840</v>
@@ -3437,7 +3453,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C170" s="5">
         <v>97020</v>
@@ -3451,7 +3467,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C171" s="5">
         <v>95320</v>
@@ -3465,7 +3481,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C172" s="5">
         <v>93930</v>
@@ -3479,7 +3495,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C173" s="5">
         <v>93920</v>
@@ -3493,7 +3509,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C174" s="5">
         <v>92300</v>
@@ -3507,7 +3523,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C175" s="5">
         <v>91490</v>
@@ -3521,7 +3537,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C176" s="5">
         <v>86700</v>
@@ -3535,7 +3551,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C177" s="5">
         <v>86230</v>
@@ -3549,7 +3565,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C178" s="5">
         <v>85540</v>
@@ -3563,7 +3579,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C179" s="5">
         <v>82270</v>
@@ -3577,7 +3593,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C180" s="5">
         <v>81630</v>
@@ -3591,7 +3607,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C181" s="5">
         <v>78000</v>
@@ -3605,7 +3621,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C182" s="5">
         <v>77360</v>
@@ -3619,7 +3635,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C183" s="5">
         <v>76860</v>
@@ -3633,7 +3649,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C184" s="5">
         <v>72320</v>
@@ -3647,7 +3663,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C185" s="5">
         <v>70980</v>
@@ -3661,7 +3677,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C186" s="5">
         <v>69060</v>
@@ -3675,7 +3691,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C187" s="5">
         <v>67170</v>
@@ -3689,7 +3705,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C188" s="5">
         <v>67150</v>
@@ -3703,7 +3719,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C189" s="5">
         <v>66710</v>
@@ -3717,7 +3733,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C190" s="5">
         <v>62840</v>
@@ -3731,7 +3747,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C191" s="5">
         <v>62360</v>
@@ -3745,7 +3761,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C192" s="5">
         <v>61460</v>
@@ -3759,7 +3775,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C193" s="5">
         <v>60220</v>
@@ -3773,7 +3789,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C194" s="5">
         <v>58410</v>
@@ -3787,7 +3803,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C195" s="5">
         <v>56980</v>
@@ -3801,7 +3817,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C196" s="5">
         <v>56660</v>
@@ -3815,7 +3831,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C197" s="5">
         <v>54100</v>
@@ -3829,7 +3845,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="C198" s="5">
         <v>53720</v>
@@ -3843,7 +3859,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C199" s="5">
         <v>52190</v>
@@ -3857,7 +3873,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C200" s="5">
         <v>49610</v>
@@ -3871,7 +3887,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C201" s="5">
         <v>42990</v>
@@ -3885,7 +3901,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C202" s="5">
         <v>42230</v>
@@ -3899,7 +3915,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C203" s="5">
         <v>35180</v>
@@ -3913,7 +3929,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C204" s="5">
         <v>31380</v>
@@ -3927,7 +3943,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C205" s="5">
         <v>30550</v>
@@ -3941,7 +3957,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C206" s="5">
         <v>27430</v>
@@ -3955,7 +3971,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C207" s="5">
         <v>25480</v>
@@ -3969,7 +3985,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C208" s="5">
         <v>24390</v>
@@ -3983,7 +3999,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C209" s="5">
         <v>15360</v>
@@ -3997,7 +4013,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C210" s="5">
         <v>13640</v>
@@ -4011,7 +4027,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C211" s="5">
         <v>4030</v>
@@ -4022,7 +4038,7 @@
     </row>
     <row r="212" spans="1:4">
       <c r="B212" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C212" s="7">
         <v>112143960</v>

</xml_diff>